<commit_message>
update segmented gait cycle rmse and add comments
</commit_message>
<xml_diff>
--- a/mode_output.xlsx
+++ b/mode_output.xlsx
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.699911090589313</v>
+        <v>2.565309470876655</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2.938666213761886</v>
+        <v>3.003081339182493</v>
       </c>
     </row>
     <row r="4">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.266772699418492</v>
+        <v>4.199891207049152</v>
       </c>
     </row>
     <row r="5">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3.425032363660399</v>
+        <v>3.274189803507521</v>
       </c>
     </row>
     <row r="6">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8.758396922038965</v>
+        <v>8.725130363174229</v>
       </c>
     </row>
     <row r="7">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.750785287564341</v>
+        <v>4.720781948531094</v>
       </c>
     </row>
     <row r="8">
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2.526569031925137</v>
+        <v>2.535127651661789</v>
       </c>
     </row>
     <row r="9">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4.968043130917457</v>
+        <v>4.809824706622224</v>
       </c>
     </row>
     <row r="10">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2.410479317143667</v>
+        <v>6.13938237555457</v>
       </c>
     </row>
     <row r="11">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.854865319528817</v>
+        <v>2.86069802887924</v>
       </c>
     </row>
     <row r="12">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2.347929327127252</v>
+        <v>2.30361538158524</v>
       </c>
     </row>
     <row r="13">
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>8.051826793850751</v>
+        <v>6.547923009847037</v>
       </c>
     </row>
     <row r="14">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.957124374769856</v>
+        <v>4.928269433743423</v>
       </c>
     </row>
     <row r="15">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>9.626635228288222</v>
+        <v>9.531842630873502</v>
       </c>
     </row>
     <row r="16">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4.676334922690037</v>
+        <v>4.323533340851341</v>
       </c>
     </row>
     <row r="17">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>18.86630957992974</v>
+        <v>12.51502503806533</v>
       </c>
     </row>
     <row r="18">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3.751705391268233</v>
+        <v>3.525476847061302</v>
       </c>
     </row>
     <row r="19">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>26.11620561538671</v>
+        <v>25.37179967584758</v>
       </c>
     </row>
     <row r="20">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>10.70214657421656</v>
+        <v>10.36424620600918</v>
       </c>
     </row>
     <row r="21">
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>7.84362082194203</v>
+        <v>9.435240225682612</v>
       </c>
     </row>
     <row r="22">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>24.78376933511203</v>
+        <v>16.09327796865148</v>
       </c>
     </row>
     <row r="23">
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>17.74066250745557</v>
+        <v>18.30366463356607</v>
       </c>
     </row>
     <row r="24">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8.926144600325934</v>
+        <v>6.111661780494481</v>
       </c>
     </row>
     <row r="25">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>16.14625162635706</v>
+        <v>16.64950296625551</v>
       </c>
     </row>
     <row r="26">
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>29.97429048711126</v>
+        <v>24.8828281198701</v>
       </c>
     </row>
     <row r="27">
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>16.80154312412373</v>
+        <v>16.1454417455465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>